<commit_message>
Implemented services and modified template importer/row handler and test templates
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/invalid_templates/Project_link_samples_v4_0_0.xlsx
+++ b/backend/fms_core/tests/invalid_templates/Project_link_samples_v4_0_0.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>Project link samples Template</t>
   </si>
@@ -50,7 +50,7 @@
     <t>Sample Container Coord</t>
   </si>
   <si>
-    <t>Add</t>
+    <t>Add to project and/or study</t>
   </si>
   <si>
     <t>ProjectTest1</t>
@@ -71,7 +71,7 @@
     <t>CONTAINER4PROJECTLINKSAMPLES2</t>
   </si>
   <si>
-    <t>Remove</t>
+    <t>Remove from project</t>
   </si>
   <si>
     <t>ProjectTest3</t>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>CONTAINER4PROJECTLINKSAMPLES3</t>
+  </si>
+  <si>
+    <t>Remove from study</t>
   </si>
 </sst>
 </file>
@@ -115,7 +118,7 @@
     <font>
       <b val="1"/>
       <sz val="11"/>
-      <color indexed="10"/>
+      <color indexed="11"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -126,7 +129,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="10"/>
+      <color indexed="11"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -150,7 +153,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="11"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -183,35 +186,35 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
@@ -228,26 +231,26 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -257,83 +260,80 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="8" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -353,12 +353,12 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffbfbfbf"/>
       <rgbColor rgb="ff92d050"/>
       <rgbColor rgb="ffffd966"/>
       <rgbColor rgb="ff6fa8dc"/>
-      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -557,12 +557,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -595,10 +595,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -846,12 +846,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1166,10 +1166,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1426,7 +1426,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
     <col min="2" max="5" width="22.3516" style="1" customWidth="1"/>
     <col min="6" max="6" width="30.5" style="1" customWidth="1"/>
     <col min="7" max="8" width="22.3516" style="1" customWidth="1"/>
@@ -1574,7 +1574,7 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" t="s" s="20">
+      <c r="A11" t="s" s="18">
         <v>19</v>
       </c>
       <c r="B11" t="s" s="19">
@@ -1607,971 +1607,971 @@
         <v>15</v>
       </c>
       <c r="G12" s="19"/>
-      <c r="H12" s="21"/>
+      <c r="H12" s="20"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="22"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
-      <c r="H13" s="21"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="22"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="21"/>
+      <c r="H14" s="20"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="22"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
-      <c r="H15" s="21"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="22"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
-      <c r="H16" s="21"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="22"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="18"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
-      <c r="H17" s="21"/>
+      <c r="H17" s="20"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="22"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
-      <c r="H18" s="21"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
-      <c r="A19" s="22"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
-      <c r="H19" s="21"/>
+      <c r="H19" s="20"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="22"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="18"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
-      <c r="H20" s="21"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="22"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
-      <c r="H21" s="21"/>
+      <c r="H21" s="20"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="22"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
-      <c r="H22" s="21"/>
+      <c r="H22" s="20"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="22"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
-      <c r="H23" s="21"/>
+      <c r="H23" s="20"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="22"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
-      <c r="H24" s="21"/>
+      <c r="H24" s="20"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="22"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="18"/>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
-      <c r="H25" s="21"/>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="22"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
-      <c r="H26" s="21"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="22"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="18"/>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
-      <c r="H27" s="21"/>
+      <c r="H27" s="20"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="22"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
-      <c r="H28" s="21"/>
+      <c r="H28" s="20"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="22"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
-      <c r="H29" s="21"/>
+      <c r="H29" s="20"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="22"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
-      <c r="H30" s="21"/>
+      <c r="H30" s="20"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="22"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="18"/>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
-      <c r="H31" s="21"/>
+      <c r="H31" s="20"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="22"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="18"/>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
-      <c r="H32" s="21"/>
+      <c r="H32" s="20"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="22"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
-      <c r="H33" s="21"/>
+      <c r="H33" s="20"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="22"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
-      <c r="H34" s="21"/>
+      <c r="H34" s="20"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="22"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="18"/>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
-      <c r="H35" s="21"/>
+      <c r="H35" s="20"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="22"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="18"/>
       <c r="C36" s="19"/>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
       <c r="F36" s="19"/>
       <c r="G36" s="19"/>
-      <c r="H36" s="21"/>
+      <c r="H36" s="20"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="22"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="18"/>
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
       <c r="E37" s="19"/>
       <c r="F37" s="19"/>
       <c r="G37" s="19"/>
-      <c r="H37" s="21"/>
+      <c r="H37" s="20"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="22"/>
+      <c r="A38" s="21"/>
       <c r="B38" s="18"/>
       <c r="C38" s="19"/>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
       <c r="G38" s="19"/>
-      <c r="H38" s="21"/>
+      <c r="H38" s="20"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="22"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="18"/>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
       <c r="E39" s="19"/>
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
-      <c r="H39" s="21"/>
+      <c r="H39" s="20"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="22"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="18"/>
       <c r="C40" s="19"/>
       <c r="D40" s="19"/>
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
       <c r="G40" s="19"/>
-      <c r="H40" s="21"/>
+      <c r="H40" s="20"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="22"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="18"/>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
       <c r="E41" s="19"/>
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
-      <c r="H41" s="21"/>
+      <c r="H41" s="20"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="22"/>
+      <c r="A42" s="21"/>
       <c r="B42" s="18"/>
       <c r="C42" s="19"/>
       <c r="D42" s="19"/>
       <c r="E42" s="19"/>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
-      <c r="H42" s="21"/>
+      <c r="H42" s="20"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="22"/>
+      <c r="A43" s="21"/>
       <c r="B43" s="18"/>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
       <c r="E43" s="19"/>
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
-      <c r="H43" s="21"/>
+      <c r="H43" s="20"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="22"/>
+      <c r="A44" s="21"/>
       <c r="B44" s="18"/>
       <c r="C44" s="19"/>
       <c r="D44" s="19"/>
       <c r="E44" s="19"/>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
-      <c r="H44" s="21"/>
+      <c r="H44" s="20"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="22"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="18"/>
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
       <c r="E45" s="19"/>
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
-      <c r="H45" s="21"/>
+      <c r="H45" s="20"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="22"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="18"/>
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
       <c r="E46" s="19"/>
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
-      <c r="H46" s="21"/>
+      <c r="H46" s="20"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="22"/>
+      <c r="A47" s="21"/>
       <c r="B47" s="18"/>
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
       <c r="E47" s="19"/>
       <c r="F47" s="19"/>
       <c r="G47" s="19"/>
-      <c r="H47" s="21"/>
+      <c r="H47" s="20"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="22"/>
+      <c r="A48" s="21"/>
       <c r="B48" s="18"/>
       <c r="C48" s="19"/>
       <c r="D48" s="19"/>
       <c r="E48" s="19"/>
       <c r="F48" s="19"/>
       <c r="G48" s="19"/>
-      <c r="H48" s="21"/>
+      <c r="H48" s="20"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="22"/>
+      <c r="A49" s="21"/>
       <c r="B49" s="18"/>
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
       <c r="E49" s="19"/>
       <c r="F49" s="19"/>
       <c r="G49" s="19"/>
-      <c r="H49" s="21"/>
+      <c r="H49" s="20"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="22"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="18"/>
       <c r="C50" s="19"/>
       <c r="D50" s="19"/>
       <c r="E50" s="19"/>
       <c r="F50" s="19"/>
       <c r="G50" s="19"/>
-      <c r="H50" s="21"/>
+      <c r="H50" s="20"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="22"/>
+      <c r="A51" s="21"/>
       <c r="B51" s="18"/>
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
       <c r="E51" s="19"/>
       <c r="F51" s="19"/>
       <c r="G51" s="19"/>
-      <c r="H51" s="21"/>
+      <c r="H51" s="20"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="22"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="18"/>
       <c r="C52" s="19"/>
       <c r="D52" s="19"/>
       <c r="E52" s="19"/>
       <c r="F52" s="19"/>
       <c r="G52" s="19"/>
-      <c r="H52" s="21"/>
+      <c r="H52" s="20"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="22"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="18"/>
       <c r="C53" s="19"/>
       <c r="D53" s="19"/>
       <c r="E53" s="19"/>
       <c r="F53" s="19"/>
       <c r="G53" s="19"/>
-      <c r="H53" s="21"/>
+      <c r="H53" s="20"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="22"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="18"/>
       <c r="C54" s="19"/>
       <c r="D54" s="19"/>
       <c r="E54" s="19"/>
       <c r="F54" s="19"/>
       <c r="G54" s="19"/>
-      <c r="H54" s="21"/>
+      <c r="H54" s="20"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="22"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="18"/>
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
       <c r="E55" s="19"/>
       <c r="F55" s="19"/>
       <c r="G55" s="19"/>
-      <c r="H55" s="21"/>
+      <c r="H55" s="20"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="22"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="18"/>
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
       <c r="E56" s="19"/>
       <c r="F56" s="19"/>
       <c r="G56" s="19"/>
-      <c r="H56" s="21"/>
+      <c r="H56" s="20"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="22"/>
+      <c r="A57" s="21"/>
       <c r="B57" s="18"/>
       <c r="C57" s="19"/>
       <c r="D57" s="19"/>
       <c r="E57" s="19"/>
       <c r="F57" s="19"/>
       <c r="G57" s="19"/>
-      <c r="H57" s="21"/>
+      <c r="H57" s="20"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="22"/>
+      <c r="A58" s="21"/>
       <c r="B58" s="18"/>
       <c r="C58" s="19"/>
       <c r="D58" s="19"/>
       <c r="E58" s="19"/>
       <c r="F58" s="19"/>
       <c r="G58" s="19"/>
-      <c r="H58" s="21"/>
+      <c r="H58" s="20"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="22"/>
+      <c r="A59" s="21"/>
       <c r="B59" s="18"/>
       <c r="C59" s="19"/>
       <c r="D59" s="19"/>
       <c r="E59" s="19"/>
       <c r="F59" s="19"/>
       <c r="G59" s="19"/>
-      <c r="H59" s="21"/>
+      <c r="H59" s="20"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="22"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="18"/>
       <c r="C60" s="19"/>
       <c r="D60" s="19"/>
       <c r="E60" s="19"/>
       <c r="F60" s="19"/>
       <c r="G60" s="19"/>
-      <c r="H60" s="21"/>
+      <c r="H60" s="20"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="22"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="18"/>
       <c r="C61" s="19"/>
       <c r="D61" s="19"/>
       <c r="E61" s="19"/>
       <c r="F61" s="19"/>
       <c r="G61" s="19"/>
-      <c r="H61" s="21"/>
+      <c r="H61" s="20"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="22"/>
+      <c r="A62" s="21"/>
       <c r="B62" s="18"/>
       <c r="C62" s="19"/>
       <c r="D62" s="19"/>
       <c r="E62" s="19"/>
       <c r="F62" s="19"/>
       <c r="G62" s="19"/>
-      <c r="H62" s="21"/>
+      <c r="H62" s="20"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="22"/>
+      <c r="A63" s="21"/>
       <c r="B63" s="18"/>
       <c r="C63" s="19"/>
       <c r="D63" s="19"/>
       <c r="E63" s="19"/>
       <c r="F63" s="19"/>
       <c r="G63" s="19"/>
-      <c r="H63" s="21"/>
+      <c r="H63" s="20"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="22"/>
+      <c r="A64" s="21"/>
       <c r="B64" s="18"/>
       <c r="C64" s="19"/>
       <c r="D64" s="19"/>
       <c r="E64" s="19"/>
       <c r="F64" s="19"/>
       <c r="G64" s="19"/>
-      <c r="H64" s="21"/>
+      <c r="H64" s="20"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="22"/>
+      <c r="A65" s="21"/>
       <c r="B65" s="18"/>
       <c r="C65" s="19"/>
       <c r="D65" s="19"/>
       <c r="E65" s="19"/>
       <c r="F65" s="19"/>
       <c r="G65" s="19"/>
-      <c r="H65" s="21"/>
+      <c r="H65" s="20"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="22"/>
+      <c r="A66" s="21"/>
       <c r="B66" s="18"/>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
       <c r="E66" s="19"/>
       <c r="F66" s="19"/>
       <c r="G66" s="19"/>
-      <c r="H66" s="21"/>
+      <c r="H66" s="20"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="22"/>
+      <c r="A67" s="21"/>
       <c r="B67" s="18"/>
       <c r="C67" s="19"/>
       <c r="D67" s="19"/>
       <c r="E67" s="19"/>
       <c r="F67" s="19"/>
       <c r="G67" s="19"/>
-      <c r="H67" s="21"/>
+      <c r="H67" s="20"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="22"/>
+      <c r="A68" s="21"/>
       <c r="B68" s="18"/>
       <c r="C68" s="19"/>
       <c r="D68" s="19"/>
       <c r="E68" s="19"/>
       <c r="F68" s="19"/>
       <c r="G68" s="19"/>
-      <c r="H68" s="21"/>
+      <c r="H68" s="20"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="22"/>
+      <c r="A69" s="21"/>
       <c r="B69" s="18"/>
       <c r="C69" s="19"/>
       <c r="D69" s="19"/>
       <c r="E69" s="19"/>
       <c r="F69" s="19"/>
       <c r="G69" s="19"/>
-      <c r="H69" s="21"/>
+      <c r="H69" s="20"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="22"/>
+      <c r="A70" s="21"/>
       <c r="B70" s="18"/>
       <c r="C70" s="19"/>
       <c r="D70" s="19"/>
       <c r="E70" s="19"/>
       <c r="F70" s="19"/>
       <c r="G70" s="19"/>
-      <c r="H70" s="21"/>
+      <c r="H70" s="20"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="22"/>
+      <c r="A71" s="21"/>
       <c r="B71" s="18"/>
       <c r="C71" s="19"/>
       <c r="D71" s="19"/>
       <c r="E71" s="19"/>
       <c r="F71" s="19"/>
       <c r="G71" s="19"/>
-      <c r="H71" s="21"/>
+      <c r="H71" s="20"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="22"/>
+      <c r="A72" s="21"/>
       <c r="B72" s="18"/>
       <c r="C72" s="19"/>
       <c r="D72" s="19"/>
       <c r="E72" s="19"/>
       <c r="F72" s="19"/>
       <c r="G72" s="19"/>
-      <c r="H72" s="21"/>
+      <c r="H72" s="20"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="22"/>
+      <c r="A73" s="21"/>
       <c r="B73" s="18"/>
       <c r="C73" s="19"/>
       <c r="D73" s="19"/>
       <c r="E73" s="19"/>
       <c r="F73" s="19"/>
       <c r="G73" s="19"/>
-      <c r="H73" s="21"/>
+      <c r="H73" s="20"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="22"/>
+      <c r="A74" s="21"/>
       <c r="B74" s="18"/>
       <c r="C74" s="19"/>
       <c r="D74" s="19"/>
       <c r="E74" s="19"/>
       <c r="F74" s="19"/>
       <c r="G74" s="19"/>
-      <c r="H74" s="21"/>
+      <c r="H74" s="20"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="22"/>
+      <c r="A75" s="21"/>
       <c r="B75" s="18"/>
       <c r="C75" s="19"/>
       <c r="D75" s="19"/>
       <c r="E75" s="19"/>
       <c r="F75" s="19"/>
       <c r="G75" s="19"/>
-      <c r="H75" s="21"/>
+      <c r="H75" s="20"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="22"/>
+      <c r="A76" s="21"/>
       <c r="B76" s="18"/>
       <c r="C76" s="19"/>
       <c r="D76" s="19"/>
       <c r="E76" s="19"/>
       <c r="F76" s="19"/>
       <c r="G76" s="19"/>
-      <c r="H76" s="21"/>
+      <c r="H76" s="20"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="22"/>
+      <c r="A77" s="21"/>
       <c r="B77" s="18"/>
       <c r="C77" s="19"/>
       <c r="D77" s="19"/>
       <c r="E77" s="19"/>
       <c r="F77" s="19"/>
       <c r="G77" s="19"/>
-      <c r="H77" s="21"/>
+      <c r="H77" s="20"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="22"/>
+      <c r="A78" s="21"/>
       <c r="B78" s="18"/>
       <c r="C78" s="19"/>
       <c r="D78" s="19"/>
       <c r="E78" s="19"/>
       <c r="F78" s="19"/>
       <c r="G78" s="19"/>
-      <c r="H78" s="21"/>
+      <c r="H78" s="20"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="22"/>
+      <c r="A79" s="21"/>
       <c r="B79" s="18"/>
       <c r="C79" s="19"/>
       <c r="D79" s="19"/>
       <c r="E79" s="19"/>
       <c r="F79" s="19"/>
       <c r="G79" s="19"/>
-      <c r="H79" s="21"/>
+      <c r="H79" s="20"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="22"/>
+      <c r="A80" s="21"/>
       <c r="B80" s="18"/>
       <c r="C80" s="19"/>
       <c r="D80" s="19"/>
       <c r="E80" s="19"/>
       <c r="F80" s="19"/>
       <c r="G80" s="19"/>
-      <c r="H80" s="21"/>
+      <c r="H80" s="20"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="22"/>
+      <c r="A81" s="21"/>
       <c r="B81" s="18"/>
       <c r="C81" s="19"/>
       <c r="D81" s="19"/>
       <c r="E81" s="19"/>
       <c r="F81" s="19"/>
       <c r="G81" s="19"/>
-      <c r="H81" s="21"/>
+      <c r="H81" s="20"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="22"/>
+      <c r="A82" s="21"/>
       <c r="B82" s="18"/>
       <c r="C82" s="19"/>
       <c r="D82" s="19"/>
       <c r="E82" s="19"/>
       <c r="F82" s="19"/>
       <c r="G82" s="19"/>
-      <c r="H82" s="21"/>
+      <c r="H82" s="20"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="22"/>
+      <c r="A83" s="21"/>
       <c r="B83" s="18"/>
       <c r="C83" s="19"/>
       <c r="D83" s="19"/>
       <c r="E83" s="19"/>
       <c r="F83" s="19"/>
       <c r="G83" s="19"/>
-      <c r="H83" s="21"/>
+      <c r="H83" s="20"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="22"/>
+      <c r="A84" s="21"/>
       <c r="B84" s="18"/>
       <c r="C84" s="19"/>
       <c r="D84" s="19"/>
       <c r="E84" s="19"/>
       <c r="F84" s="19"/>
       <c r="G84" s="19"/>
-      <c r="H84" s="21"/>
+      <c r="H84" s="20"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="22"/>
+      <c r="A85" s="21"/>
       <c r="B85" s="18"/>
       <c r="C85" s="19"/>
       <c r="D85" s="19"/>
       <c r="E85" s="19"/>
       <c r="F85" s="19"/>
       <c r="G85" s="19"/>
-      <c r="H85" s="21"/>
+      <c r="H85" s="20"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="22"/>
+      <c r="A86" s="21"/>
       <c r="B86" s="18"/>
       <c r="C86" s="19"/>
       <c r="D86" s="19"/>
       <c r="E86" s="19"/>
       <c r="F86" s="19"/>
       <c r="G86" s="19"/>
-      <c r="H86" s="21"/>
+      <c r="H86" s="20"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="22"/>
+      <c r="A87" s="21"/>
       <c r="B87" s="18"/>
       <c r="C87" s="19"/>
       <c r="D87" s="19"/>
       <c r="E87" s="19"/>
       <c r="F87" s="19"/>
       <c r="G87" s="19"/>
-      <c r="H87" s="21"/>
+      <c r="H87" s="20"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="22"/>
+      <c r="A88" s="21"/>
       <c r="B88" s="18"/>
       <c r="C88" s="19"/>
       <c r="D88" s="19"/>
       <c r="E88" s="19"/>
       <c r="F88" s="19"/>
       <c r="G88" s="19"/>
-      <c r="H88" s="21"/>
+      <c r="H88" s="20"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="22"/>
+      <c r="A89" s="21"/>
       <c r="B89" s="18"/>
       <c r="C89" s="19"/>
       <c r="D89" s="19"/>
       <c r="E89" s="19"/>
       <c r="F89" s="19"/>
       <c r="G89" s="19"/>
-      <c r="H89" s="21"/>
+      <c r="H89" s="20"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="22"/>
+      <c r="A90" s="21"/>
       <c r="B90" s="18"/>
       <c r="C90" s="19"/>
       <c r="D90" s="19"/>
       <c r="E90" s="19"/>
       <c r="F90" s="19"/>
       <c r="G90" s="19"/>
-      <c r="H90" s="21"/>
+      <c r="H90" s="20"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="22"/>
+      <c r="A91" s="21"/>
       <c r="B91" s="18"/>
       <c r="C91" s="19"/>
       <c r="D91" s="19"/>
       <c r="E91" s="19"/>
       <c r="F91" s="19"/>
       <c r="G91" s="19"/>
-      <c r="H91" s="21"/>
+      <c r="H91" s="20"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="22"/>
+      <c r="A92" s="21"/>
       <c r="B92" s="18"/>
       <c r="C92" s="19"/>
       <c r="D92" s="19"/>
       <c r="E92" s="19"/>
       <c r="F92" s="19"/>
       <c r="G92" s="19"/>
-      <c r="H92" s="21"/>
+      <c r="H92" s="20"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="22"/>
+      <c r="A93" s="21"/>
       <c r="B93" s="18"/>
       <c r="C93" s="19"/>
       <c r="D93" s="19"/>
       <c r="E93" s="19"/>
       <c r="F93" s="19"/>
       <c r="G93" s="19"/>
-      <c r="H93" s="21"/>
+      <c r="H93" s="20"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="22"/>
+      <c r="A94" s="21"/>
       <c r="B94" s="18"/>
       <c r="C94" s="19"/>
       <c r="D94" s="19"/>
       <c r="E94" s="19"/>
       <c r="F94" s="19"/>
       <c r="G94" s="19"/>
-      <c r="H94" s="21"/>
+      <c r="H94" s="20"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="22"/>
+      <c r="A95" s="21"/>
       <c r="B95" s="18"/>
       <c r="C95" s="19"/>
       <c r="D95" s="19"/>
       <c r="E95" s="19"/>
       <c r="F95" s="19"/>
       <c r="G95" s="19"/>
-      <c r="H95" s="21"/>
+      <c r="H95" s="20"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="22"/>
+      <c r="A96" s="21"/>
       <c r="B96" s="18"/>
       <c r="C96" s="19"/>
       <c r="D96" s="19"/>
       <c r="E96" s="19"/>
       <c r="F96" s="19"/>
       <c r="G96" s="19"/>
-      <c r="H96" s="21"/>
+      <c r="H96" s="20"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="22"/>
+      <c r="A97" s="21"/>
       <c r="B97" s="18"/>
       <c r="C97" s="19"/>
       <c r="D97" s="19"/>
       <c r="E97" s="19"/>
       <c r="F97" s="19"/>
       <c r="G97" s="19"/>
-      <c r="H97" s="21"/>
+      <c r="H97" s="20"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="22"/>
+      <c r="A98" s="21"/>
       <c r="B98" s="18"/>
       <c r="C98" s="19"/>
       <c r="D98" s="19"/>
       <c r="E98" s="19"/>
       <c r="F98" s="19"/>
       <c r="G98" s="19"/>
-      <c r="H98" s="21"/>
+      <c r="H98" s="20"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="22"/>
+      <c r="A99" s="21"/>
       <c r="B99" s="18"/>
       <c r="C99" s="19"/>
       <c r="D99" s="19"/>
       <c r="E99" s="19"/>
       <c r="F99" s="19"/>
       <c r="G99" s="19"/>
-      <c r="H99" s="21"/>
+      <c r="H99" s="20"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="22"/>
+      <c r="A100" s="21"/>
       <c r="B100" s="18"/>
       <c r="C100" s="19"/>
       <c r="D100" s="19"/>
       <c r="E100" s="19"/>
       <c r="F100" s="19"/>
       <c r="G100" s="19"/>
-      <c r="H100" s="21"/>
+      <c r="H100" s="20"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="22"/>
+      <c r="A101" s="21"/>
       <c r="B101" s="18"/>
       <c r="C101" s="19"/>
       <c r="D101" s="19"/>
       <c r="E101" s="19"/>
       <c r="F101" s="19"/>
       <c r="G101" s="19"/>
-      <c r="H101" s="21"/>
+      <c r="H101" s="20"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="22"/>
+      <c r="A102" s="21"/>
       <c r="B102" s="18"/>
       <c r="C102" s="19"/>
       <c r="D102" s="19"/>
       <c r="E102" s="19"/>
       <c r="F102" s="19"/>
       <c r="G102" s="19"/>
-      <c r="H102" s="21"/>
+      <c r="H102" s="20"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="22"/>
+      <c r="A103" s="21"/>
       <c r="B103" s="18"/>
       <c r="C103" s="19"/>
       <c r="D103" s="19"/>
       <c r="E103" s="19"/>
       <c r="F103" s="19"/>
       <c r="G103" s="19"/>
-      <c r="H103" s="21"/>
+      <c r="H103" s="20"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="22"/>
+      <c r="A104" s="21"/>
       <c r="B104" s="18"/>
       <c r="C104" s="19"/>
       <c r="D104" s="19"/>
       <c r="E104" s="19"/>
       <c r="F104" s="19"/>
       <c r="G104" s="19"/>
-      <c r="H104" s="21"/>
+      <c r="H104" s="20"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="22"/>
+      <c r="A105" s="21"/>
       <c r="B105" s="18"/>
       <c r="C105" s="19"/>
       <c r="D105" s="19"/>
       <c r="E105" s="19"/>
       <c r="F105" s="19"/>
       <c r="G105" s="19"/>
-      <c r="H105" s="21"/>
+      <c r="H105" s="20"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="22"/>
-      <c r="B106" s="23"/>
-      <c r="C106" s="21"/>
-      <c r="D106" s="21"/>
-      <c r="E106" s="21"/>
-      <c r="F106" s="21"/>
-      <c r="G106" s="21"/>
-      <c r="H106" s="21"/>
+      <c r="A106" s="21"/>
+      <c r="B106" s="21"/>
+      <c r="C106" s="20"/>
+      <c r="D106" s="20"/>
+      <c r="E106" s="20"/>
+      <c r="F106" s="20"/>
+      <c r="G106" s="20"/>
+      <c r="H106" s="20"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="22"/>
-      <c r="B107" s="23"/>
-      <c r="C107" s="21"/>
-      <c r="D107" s="21"/>
-      <c r="E107" s="21"/>
-      <c r="F107" s="21"/>
-      <c r="G107" s="21"/>
-      <c r="H107" s="21"/>
+      <c r="A107" s="21"/>
+      <c r="B107" s="21"/>
+      <c r="C107" s="20"/>
+      <c r="D107" s="20"/>
+      <c r="E107" s="20"/>
+      <c r="F107" s="20"/>
+      <c r="G107" s="20"/>
+      <c r="H107" s="20"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="22"/>
-      <c r="B108" s="23"/>
-      <c r="C108" s="21"/>
-      <c r="D108" s="21"/>
-      <c r="E108" s="21"/>
-      <c r="F108" s="21"/>
-      <c r="G108" s="21"/>
-      <c r="H108" s="21"/>
+      <c r="A108" s="21"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="20"/>
+      <c r="D108" s="20"/>
+      <c r="E108" s="20"/>
+      <c r="F108" s="20"/>
+      <c r="G108" s="20"/>
+      <c r="H108" s="20"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="22"/>
-      <c r="B109" s="23"/>
+      <c r="A109" s="21"/>
+      <c r="B109" s="21"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
@@ -2580,8 +2580,8 @@
       <c r="H109" s="4"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="22"/>
-      <c r="B110" s="23"/>
+      <c r="A110" s="21"/>
+      <c r="B110" s="21"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
@@ -2590,8 +2590,8 @@
       <c r="H110" s="4"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="22"/>
-      <c r="B111" s="23"/>
+      <c r="A111" s="21"/>
+      <c r="B111" s="21"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -2600,8 +2600,8 @@
       <c r="H111" s="4"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="22"/>
-      <c r="B112" s="23"/>
+      <c r="A112" s="21"/>
+      <c r="B112" s="21"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -2610,8 +2610,8 @@
       <c r="H112" s="4"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="22"/>
-      <c r="B113" s="23"/>
+      <c r="A113" s="21"/>
+      <c r="B113" s="21"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -2620,8 +2620,8 @@
       <c r="H113" s="4"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="22"/>
-      <c r="B114" s="23"/>
+      <c r="A114" s="21"/>
+      <c r="B114" s="21"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
@@ -2630,8 +2630,8 @@
       <c r="H114" s="4"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="22"/>
-      <c r="B115" s="23"/>
+      <c r="A115" s="21"/>
+      <c r="B115" s="21"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
@@ -2640,8 +2640,8 @@
       <c r="H115" s="4"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="22"/>
-      <c r="B116" s="23"/>
+      <c r="A116" s="21"/>
+      <c r="B116" s="21"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
@@ -2650,8 +2650,8 @@
       <c r="H116" s="4"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="22"/>
-      <c r="B117" s="23"/>
+      <c r="A117" s="21"/>
+      <c r="B117" s="21"/>
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -2660,8 +2660,8 @@
       <c r="H117" s="4"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="22"/>
-      <c r="B118" s="23"/>
+      <c r="A118" s="21"/>
+      <c r="B118" s="21"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -2670,8 +2670,8 @@
       <c r="H118" s="4"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="22"/>
-      <c r="B119" s="23"/>
+      <c r="A119" s="21"/>
+      <c r="B119" s="21"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
@@ -2680,8 +2680,8 @@
       <c r="H119" s="4"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="22"/>
-      <c r="B120" s="23"/>
+      <c r="A120" s="21"/>
+      <c r="B120" s="21"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
@@ -2691,7 +2691,7 @@
     </row>
     <row r="121" ht="15.75" customHeight="1">
       <c r="A121" s="22"/>
-      <c r="B121" s="23"/>
+      <c r="B121" s="21"/>
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
@@ -2701,7 +2701,7 @@
     </row>
     <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="22"/>
-      <c r="B122" s="23"/>
+      <c r="B122" s="21"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
@@ -2711,7 +2711,7 @@
     </row>
     <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="22"/>
-      <c r="B123" s="23"/>
+      <c r="B123" s="21"/>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
@@ -2721,7 +2721,7 @@
     </row>
     <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="22"/>
-      <c r="B124" s="23"/>
+      <c r="B124" s="21"/>
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="22"/>
-      <c r="B125" s="23"/>
+      <c r="B125" s="21"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
@@ -2741,7 +2741,7 @@
     </row>
     <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="22"/>
-      <c r="B126" s="23"/>
+      <c r="B126" s="21"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
@@ -2751,7 +2751,7 @@
     </row>
     <row r="127" ht="15.75" customHeight="1">
       <c r="A127" s="22"/>
-      <c r="B127" s="23"/>
+      <c r="B127" s="21"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
@@ -2761,7 +2761,7 @@
     </row>
     <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="22"/>
-      <c r="B128" s="23"/>
+      <c r="B128" s="21"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
@@ -2771,7 +2771,7 @@
     </row>
     <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="22"/>
-      <c r="B129" s="23"/>
+      <c r="B129" s="21"/>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
@@ -2781,7 +2781,7 @@
     </row>
     <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="22"/>
-      <c r="B130" s="23"/>
+      <c r="B130" s="21"/>
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
       <c r="E130" s="4"/>
@@ -2791,7 +2791,7 @@
     </row>
     <row r="131" ht="15.75" customHeight="1">
       <c r="A131" s="22"/>
-      <c r="B131" s="23"/>
+      <c r="B131" s="21"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
       <c r="E131" s="4"/>
@@ -2801,7 +2801,7 @@
     </row>
     <row r="132" ht="15.75" customHeight="1">
       <c r="A132" s="22"/>
-      <c r="B132" s="23"/>
+      <c r="B132" s="21"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="133" ht="15.75" customHeight="1">
       <c r="A133" s="22"/>
-      <c r="B133" s="23"/>
+      <c r="B133" s="21"/>
       <c r="C133" s="4"/>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
@@ -2821,7 +2821,7 @@
     </row>
     <row r="134" ht="15.75" customHeight="1">
       <c r="A134" s="22"/>
-      <c r="B134" s="23"/>
+      <c r="B134" s="21"/>
       <c r="C134" s="4"/>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
@@ -2831,7 +2831,7 @@
     </row>
     <row r="135" ht="15.75" customHeight="1">
       <c r="A135" s="22"/>
-      <c r="B135" s="23"/>
+      <c r="B135" s="21"/>
       <c r="C135" s="4"/>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
@@ -2841,7 +2841,7 @@
     </row>
     <row r="136" ht="15.75" customHeight="1">
       <c r="A136" s="22"/>
-      <c r="B136" s="23"/>
+      <c r="B136" s="21"/>
       <c r="C136" s="4"/>
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
@@ -2851,7 +2851,7 @@
     </row>
     <row r="137" ht="15.75" customHeight="1">
       <c r="A137" s="22"/>
-      <c r="B137" s="23"/>
+      <c r="B137" s="21"/>
       <c r="C137" s="4"/>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
@@ -2861,7 +2861,7 @@
     </row>
     <row r="138" ht="15.75" customHeight="1">
       <c r="A138" s="22"/>
-      <c r="B138" s="23"/>
+      <c r="B138" s="21"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
@@ -2871,7 +2871,7 @@
     </row>
     <row r="139" ht="15.75" customHeight="1">
       <c r="A139" s="22"/>
-      <c r="B139" s="23"/>
+      <c r="B139" s="21"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
@@ -2881,7 +2881,7 @@
     </row>
     <row r="140" ht="15.75" customHeight="1">
       <c r="A140" s="22"/>
-      <c r="B140" s="23"/>
+      <c r="B140" s="21"/>
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="141" ht="15.75" customHeight="1">
       <c r="A141" s="22"/>
-      <c r="B141" s="23"/>
+      <c r="B141" s="21"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
@@ -2901,7 +2901,7 @@
     </row>
     <row r="142" ht="15.75" customHeight="1">
       <c r="A142" s="22"/>
-      <c r="B142" s="23"/>
+      <c r="B142" s="21"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
       <c r="E142" s="4"/>
@@ -2911,7 +2911,7 @@
     </row>
     <row r="143" ht="15.75" customHeight="1">
       <c r="A143" s="22"/>
-      <c r="B143" s="23"/>
+      <c r="B143" s="21"/>
       <c r="C143" s="4"/>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
@@ -2921,7 +2921,7 @@
     </row>
     <row r="144" ht="15.75" customHeight="1">
       <c r="A144" s="22"/>
-      <c r="B144" s="23"/>
+      <c r="B144" s="21"/>
       <c r="C144" s="4"/>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="145" ht="15.75" customHeight="1">
       <c r="A145" s="22"/>
-      <c r="B145" s="23"/>
+      <c r="B145" s="21"/>
       <c r="C145" s="4"/>
       <c r="D145" s="4"/>
       <c r="E145" s="4"/>
@@ -2941,7 +2941,7 @@
     </row>
     <row r="146" ht="15.75" customHeight="1">
       <c r="A146" s="22"/>
-      <c r="B146" s="23"/>
+      <c r="B146" s="21"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
@@ -2951,7 +2951,7 @@
     </row>
     <row r="147" ht="15.75" customHeight="1">
       <c r="A147" s="22"/>
-      <c r="B147" s="23"/>
+      <c r="B147" s="21"/>
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
@@ -2961,7 +2961,7 @@
     </row>
     <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="22"/>
-      <c r="B148" s="23"/>
+      <c r="B148" s="21"/>
       <c r="C148" s="4"/>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="149" ht="15.75" customHeight="1">
       <c r="A149" s="22"/>
-      <c r="B149" s="23"/>
+      <c r="B149" s="21"/>
       <c r="C149" s="4"/>
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
@@ -2981,7 +2981,7 @@
     </row>
     <row r="150" ht="15.75" customHeight="1">
       <c r="A150" s="22"/>
-      <c r="B150" s="23"/>
+      <c r="B150" s="21"/>
       <c r="C150" s="4"/>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
@@ -2991,7 +2991,7 @@
     </row>
     <row r="151" ht="15.75" customHeight="1">
       <c r="A151" s="22"/>
-      <c r="B151" s="23"/>
+      <c r="B151" s="21"/>
       <c r="C151" s="4"/>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
@@ -3001,7 +3001,7 @@
     </row>
     <row r="152" ht="15.75" customHeight="1">
       <c r="A152" s="22"/>
-      <c r="B152" s="23"/>
+      <c r="B152" s="21"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
@@ -3011,7 +3011,7 @@
     </row>
     <row r="153" ht="15.75" customHeight="1">
       <c r="A153" s="22"/>
-      <c r="B153" s="23"/>
+      <c r="B153" s="21"/>
       <c r="C153" s="4"/>
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
@@ -3021,7 +3021,7 @@
     </row>
     <row r="154" ht="15.75" customHeight="1">
       <c r="A154" s="22"/>
-      <c r="B154" s="23"/>
+      <c r="B154" s="21"/>
       <c r="C154" s="4"/>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
@@ -3031,7 +3031,7 @@
     </row>
     <row r="155" ht="15.75" customHeight="1">
       <c r="A155" s="22"/>
-      <c r="B155" s="23"/>
+      <c r="B155" s="21"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
@@ -3041,7 +3041,7 @@
     </row>
     <row r="156" ht="15.75" customHeight="1">
       <c r="A156" s="22"/>
-      <c r="B156" s="23"/>
+      <c r="B156" s="21"/>
       <c r="C156" s="4"/>
       <c r="D156" s="4"/>
       <c r="E156" s="4"/>
@@ -3051,7 +3051,7 @@
     </row>
     <row r="157" ht="15.75" customHeight="1">
       <c r="A157" s="22"/>
-      <c r="B157" s="23"/>
+      <c r="B157" s="21"/>
       <c r="C157" s="4"/>
       <c r="D157" s="4"/>
       <c r="E157" s="4"/>
@@ -3061,7 +3061,7 @@
     </row>
     <row r="158" ht="15.75" customHeight="1">
       <c r="A158" s="22"/>
-      <c r="B158" s="23"/>
+      <c r="B158" s="21"/>
       <c r="C158" s="4"/>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
@@ -3071,7 +3071,7 @@
     </row>
     <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="22"/>
-      <c r="B159" s="23"/>
+      <c r="B159" s="21"/>
       <c r="C159" s="4"/>
       <c r="D159" s="4"/>
       <c r="E159" s="4"/>
@@ -3081,7 +3081,7 @@
     </row>
     <row r="160" ht="15.75" customHeight="1">
       <c r="A160" s="22"/>
-      <c r="B160" s="23"/>
+      <c r="B160" s="21"/>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
       <c r="E160" s="4"/>
@@ -3091,7 +3091,7 @@
     </row>
     <row r="161" ht="15.75" customHeight="1">
       <c r="A161" s="22"/>
-      <c r="B161" s="23"/>
+      <c r="B161" s="21"/>
       <c r="C161" s="4"/>
       <c r="D161" s="4"/>
       <c r="E161" s="4"/>
@@ -3101,7 +3101,7 @@
     </row>
     <row r="162" ht="15.75" customHeight="1">
       <c r="A162" s="22"/>
-      <c r="B162" s="23"/>
+      <c r="B162" s="21"/>
       <c r="C162" s="4"/>
       <c r="D162" s="4"/>
       <c r="E162" s="4"/>
@@ -3111,7 +3111,7 @@
     </row>
     <row r="163" ht="15.75" customHeight="1">
       <c r="A163" s="22"/>
-      <c r="B163" s="23"/>
+      <c r="B163" s="21"/>
       <c r="C163" s="4"/>
       <c r="D163" s="4"/>
       <c r="E163" s="4"/>
@@ -3121,7 +3121,7 @@
     </row>
     <row r="164" ht="15.75" customHeight="1">
       <c r="A164" s="22"/>
-      <c r="B164" s="23"/>
+      <c r="B164" s="21"/>
       <c r="C164" s="4"/>
       <c r="D164" s="4"/>
       <c r="E164" s="4"/>
@@ -3131,7 +3131,7 @@
     </row>
     <row r="165" ht="15.75" customHeight="1">
       <c r="A165" s="22"/>
-      <c r="B165" s="23"/>
+      <c r="B165" s="21"/>
       <c r="C165" s="4"/>
       <c r="D165" s="4"/>
       <c r="E165" s="4"/>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="166" ht="15.75" customHeight="1">
       <c r="A166" s="22"/>
-      <c r="B166" s="23"/>
+      <c r="B166" s="21"/>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
       <c r="E166" s="4"/>
@@ -3151,7 +3151,7 @@
     </row>
     <row r="167" ht="15.75" customHeight="1">
       <c r="A167" s="22"/>
-      <c r="B167" s="23"/>
+      <c r="B167" s="21"/>
       <c r="C167" s="4"/>
       <c r="D167" s="4"/>
       <c r="E167" s="4"/>
@@ -3161,7 +3161,7 @@
     </row>
     <row r="168" ht="15.75" customHeight="1">
       <c r="A168" s="22"/>
-      <c r="B168" s="23"/>
+      <c r="B168" s="21"/>
       <c r="C168" s="4"/>
       <c r="D168" s="4"/>
       <c r="E168" s="4"/>
@@ -3171,7 +3171,7 @@
     </row>
     <row r="169" ht="15.75" customHeight="1">
       <c r="A169" s="22"/>
-      <c r="B169" s="23"/>
+      <c r="B169" s="21"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
       <c r="E169" s="4"/>
@@ -3181,7 +3181,7 @@
     </row>
     <row r="170" ht="15.75" customHeight="1">
       <c r="A170" s="22"/>
-      <c r="B170" s="23"/>
+      <c r="B170" s="21"/>
       <c r="C170" s="4"/>
       <c r="D170" s="4"/>
       <c r="E170" s="4"/>
@@ -3191,7 +3191,7 @@
     </row>
     <row r="171" ht="15.75" customHeight="1">
       <c r="A171" s="22"/>
-      <c r="B171" s="23"/>
+      <c r="B171" s="21"/>
       <c r="C171" s="4"/>
       <c r="D171" s="4"/>
       <c r="E171" s="4"/>
@@ -3201,7 +3201,7 @@
     </row>
     <row r="172" ht="15.75" customHeight="1">
       <c r="A172" s="22"/>
-      <c r="B172" s="23"/>
+      <c r="B172" s="21"/>
       <c r="C172" s="4"/>
       <c r="D172" s="4"/>
       <c r="E172" s="4"/>
@@ -3211,7 +3211,7 @@
     </row>
     <row r="173" ht="15.75" customHeight="1">
       <c r="A173" s="22"/>
-      <c r="B173" s="23"/>
+      <c r="B173" s="21"/>
       <c r="C173" s="4"/>
       <c r="D173" s="4"/>
       <c r="E173" s="4"/>
@@ -3221,7 +3221,7 @@
     </row>
     <row r="174" ht="15.75" customHeight="1">
       <c r="A174" s="22"/>
-      <c r="B174" s="23"/>
+      <c r="B174" s="21"/>
       <c r="C174" s="4"/>
       <c r="D174" s="4"/>
       <c r="E174" s="4"/>
@@ -3231,7 +3231,7 @@
     </row>
     <row r="175" ht="15.75" customHeight="1">
       <c r="A175" s="22"/>
-      <c r="B175" s="23"/>
+      <c r="B175" s="21"/>
       <c r="C175" s="4"/>
       <c r="D175" s="4"/>
       <c r="E175" s="4"/>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="176" ht="15.75" customHeight="1">
       <c r="A176" s="22"/>
-      <c r="B176" s="23"/>
+      <c r="B176" s="21"/>
       <c r="C176" s="4"/>
       <c r="D176" s="4"/>
       <c r="E176" s="4"/>
@@ -3251,7 +3251,7 @@
     </row>
     <row r="177" ht="15.75" customHeight="1">
       <c r="A177" s="22"/>
-      <c r="B177" s="23"/>
+      <c r="B177" s="21"/>
       <c r="C177" s="4"/>
       <c r="D177" s="4"/>
       <c r="E177" s="4"/>
@@ -3261,7 +3261,7 @@
     </row>
     <row r="178" ht="15.75" customHeight="1">
       <c r="A178" s="22"/>
-      <c r="B178" s="23"/>
+      <c r="B178" s="21"/>
       <c r="C178" s="4"/>
       <c r="D178" s="4"/>
       <c r="E178" s="4"/>
@@ -3271,7 +3271,7 @@
     </row>
     <row r="179" ht="15.75" customHeight="1">
       <c r="A179" s="22"/>
-      <c r="B179" s="23"/>
+      <c r="B179" s="21"/>
       <c r="C179" s="4"/>
       <c r="D179" s="4"/>
       <c r="E179" s="4"/>
@@ -3281,7 +3281,7 @@
     </row>
     <row r="180" ht="15.75" customHeight="1">
       <c r="A180" s="22"/>
-      <c r="B180" s="23"/>
+      <c r="B180" s="21"/>
       <c r="C180" s="4"/>
       <c r="D180" s="4"/>
       <c r="E180" s="4"/>
@@ -3291,7 +3291,7 @@
     </row>
     <row r="181" ht="15.75" customHeight="1">
       <c r="A181" s="22"/>
-      <c r="B181" s="23"/>
+      <c r="B181" s="21"/>
       <c r="C181" s="4"/>
       <c r="D181" s="4"/>
       <c r="E181" s="4"/>
@@ -3301,7 +3301,7 @@
     </row>
     <row r="182" ht="15.75" customHeight="1">
       <c r="A182" s="22"/>
-      <c r="B182" s="23"/>
+      <c r="B182" s="21"/>
       <c r="C182" s="4"/>
       <c r="D182" s="4"/>
       <c r="E182" s="4"/>
@@ -3311,7 +3311,7 @@
     </row>
     <row r="183" ht="15.75" customHeight="1">
       <c r="A183" s="22"/>
-      <c r="B183" s="23"/>
+      <c r="B183" s="21"/>
       <c r="C183" s="4"/>
       <c r="D183" s="4"/>
       <c r="E183" s="4"/>
@@ -3321,7 +3321,7 @@
     </row>
     <row r="184" ht="15.75" customHeight="1">
       <c r="A184" s="22"/>
-      <c r="B184" s="23"/>
+      <c r="B184" s="21"/>
       <c r="C184" s="4"/>
       <c r="D184" s="4"/>
       <c r="E184" s="4"/>
@@ -3331,7 +3331,7 @@
     </row>
     <row r="185" ht="15.75" customHeight="1">
       <c r="A185" s="22"/>
-      <c r="B185" s="23"/>
+      <c r="B185" s="21"/>
       <c r="C185" s="4"/>
       <c r="D185" s="4"/>
       <c r="E185" s="4"/>
@@ -3341,7 +3341,7 @@
     </row>
     <row r="186" ht="15.75" customHeight="1">
       <c r="A186" s="22"/>
-      <c r="B186" s="23"/>
+      <c r="B186" s="21"/>
       <c r="C186" s="4"/>
       <c r="D186" s="4"/>
       <c r="E186" s="4"/>
@@ -3351,7 +3351,7 @@
     </row>
     <row r="187" ht="15.75" customHeight="1">
       <c r="A187" s="22"/>
-      <c r="B187" s="23"/>
+      <c r="B187" s="21"/>
       <c r="C187" s="4"/>
       <c r="D187" s="4"/>
       <c r="E187" s="4"/>
@@ -3361,7 +3361,7 @@
     </row>
     <row r="188" ht="15.75" customHeight="1">
       <c r="A188" s="22"/>
-      <c r="B188" s="23"/>
+      <c r="B188" s="21"/>
       <c r="C188" s="4"/>
       <c r="D188" s="4"/>
       <c r="E188" s="4"/>
@@ -3371,7 +3371,7 @@
     </row>
     <row r="189" ht="15.75" customHeight="1">
       <c r="A189" s="22"/>
-      <c r="B189" s="23"/>
+      <c r="B189" s="21"/>
       <c r="C189" s="4"/>
       <c r="D189" s="4"/>
       <c r="E189" s="4"/>
@@ -3381,7 +3381,7 @@
     </row>
     <row r="190" ht="15.75" customHeight="1">
       <c r="A190" s="22"/>
-      <c r="B190" s="23"/>
+      <c r="B190" s="21"/>
       <c r="C190" s="4"/>
       <c r="D190" s="4"/>
       <c r="E190" s="4"/>
@@ -3391,7 +3391,7 @@
     </row>
     <row r="191" ht="15.75" customHeight="1">
       <c r="A191" s="22"/>
-      <c r="B191" s="23"/>
+      <c r="B191" s="21"/>
       <c r="C191" s="4"/>
       <c r="D191" s="4"/>
       <c r="E191" s="4"/>
@@ -3401,7 +3401,7 @@
     </row>
     <row r="192" ht="15.75" customHeight="1">
       <c r="A192" s="22"/>
-      <c r="B192" s="23"/>
+      <c r="B192" s="21"/>
       <c r="C192" s="4"/>
       <c r="D192" s="4"/>
       <c r="E192" s="4"/>
@@ -3411,7 +3411,7 @@
     </row>
     <row r="193" ht="15.75" customHeight="1">
       <c r="A193" s="22"/>
-      <c r="B193" s="23"/>
+      <c r="B193" s="21"/>
       <c r="C193" s="4"/>
       <c r="D193" s="4"/>
       <c r="E193" s="4"/>
@@ -3421,7 +3421,7 @@
     </row>
     <row r="194" ht="15.75" customHeight="1">
       <c r="A194" s="22"/>
-      <c r="B194" s="23"/>
+      <c r="B194" s="21"/>
       <c r="C194" s="4"/>
       <c r="D194" s="4"/>
       <c r="E194" s="4"/>
@@ -3431,7 +3431,7 @@
     </row>
     <row r="195" ht="15.75" customHeight="1">
       <c r="A195" s="22"/>
-      <c r="B195" s="23"/>
+      <c r="B195" s="21"/>
       <c r="C195" s="4"/>
       <c r="D195" s="4"/>
       <c r="E195" s="4"/>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="196" ht="15.75" customHeight="1">
       <c r="A196" s="22"/>
-      <c r="B196" s="23"/>
+      <c r="B196" s="21"/>
       <c r="C196" s="4"/>
       <c r="D196" s="4"/>
       <c r="E196" s="4"/>
@@ -3451,7 +3451,7 @@
     </row>
     <row r="197" ht="15.75" customHeight="1">
       <c r="A197" s="22"/>
-      <c r="B197" s="23"/>
+      <c r="B197" s="21"/>
       <c r="C197" s="4"/>
       <c r="D197" s="4"/>
       <c r="E197" s="4"/>
@@ -3461,7 +3461,7 @@
     </row>
     <row r="198" ht="15.75" customHeight="1">
       <c r="A198" s="22"/>
-      <c r="B198" s="23"/>
+      <c r="B198" s="21"/>
       <c r="C198" s="4"/>
       <c r="D198" s="4"/>
       <c r="E198" s="4"/>
@@ -3471,7 +3471,7 @@
     </row>
     <row r="199" ht="15.75" customHeight="1">
       <c r="A199" s="22"/>
-      <c r="B199" s="23"/>
+      <c r="B199" s="21"/>
       <c r="C199" s="4"/>
       <c r="D199" s="4"/>
       <c r="E199" s="4"/>
@@ -3481,7 +3481,7 @@
     </row>
     <row r="200" ht="15.75" customHeight="1">
       <c r="A200" s="22"/>
-      <c r="B200" s="23"/>
+      <c r="B200" s="21"/>
       <c r="C200" s="4"/>
       <c r="D200" s="4"/>
       <c r="E200" s="4"/>
@@ -3491,7 +3491,7 @@
     </row>
     <row r="201" ht="15.75" customHeight="1">
       <c r="A201" s="22"/>
-      <c r="B201" s="23"/>
+      <c r="B201" s="21"/>
       <c r="C201" s="4"/>
       <c r="D201" s="4"/>
       <c r="E201" s="4"/>
@@ -3501,7 +3501,7 @@
     </row>
     <row r="202" ht="15.75" customHeight="1">
       <c r="A202" s="22"/>
-      <c r="B202" s="23"/>
+      <c r="B202" s="21"/>
       <c r="C202" s="4"/>
       <c r="D202" s="4"/>
       <c r="E202" s="4"/>
@@ -3511,7 +3511,7 @@
     </row>
     <row r="203" ht="15.75" customHeight="1">
       <c r="A203" s="22"/>
-      <c r="B203" s="23"/>
+      <c r="B203" s="21"/>
       <c r="C203" s="4"/>
       <c r="D203" s="4"/>
       <c r="E203" s="4"/>
@@ -3521,7 +3521,7 @@
     </row>
     <row r="204" ht="15.75" customHeight="1">
       <c r="A204" s="22"/>
-      <c r="B204" s="23"/>
+      <c r="B204" s="21"/>
       <c r="C204" s="4"/>
       <c r="D204" s="4"/>
       <c r="E204" s="4"/>
@@ -3531,7 +3531,7 @@
     </row>
     <row r="205" ht="15.75" customHeight="1">
       <c r="A205" s="22"/>
-      <c r="B205" s="23"/>
+      <c r="B205" s="21"/>
       <c r="C205" s="4"/>
       <c r="D205" s="4"/>
       <c r="E205" s="4"/>
@@ -3541,7 +3541,7 @@
     </row>
     <row r="206" ht="15.75" customHeight="1">
       <c r="A206" s="22"/>
-      <c r="B206" s="23"/>
+      <c r="B206" s="21"/>
       <c r="C206" s="4"/>
       <c r="D206" s="4"/>
       <c r="E206" s="4"/>
@@ -3551,7 +3551,7 @@
     </row>
     <row r="207" ht="15.75" customHeight="1">
       <c r="A207" s="22"/>
-      <c r="B207" s="23"/>
+      <c r="B207" s="21"/>
       <c r="C207" s="4"/>
       <c r="D207" s="4"/>
       <c r="E207" s="4"/>
@@ -3561,7 +3561,7 @@
     </row>
     <row r="208" ht="15.75" customHeight="1">
       <c r="A208" s="22"/>
-      <c r="B208" s="23"/>
+      <c r="B208" s="21"/>
       <c r="C208" s="4"/>
       <c r="D208" s="4"/>
       <c r="E208" s="4"/>
@@ -3571,7 +3571,7 @@
     </row>
     <row r="209" ht="15.75" customHeight="1">
       <c r="A209" s="22"/>
-      <c r="B209" s="23"/>
+      <c r="B209" s="21"/>
       <c r="C209" s="4"/>
       <c r="D209" s="4"/>
       <c r="E209" s="4"/>
@@ -3581,7 +3581,7 @@
     </row>
     <row r="210" ht="15.75" customHeight="1">
       <c r="A210" s="22"/>
-      <c r="B210" s="23"/>
+      <c r="B210" s="21"/>
       <c r="C210" s="4"/>
       <c r="D210" s="4"/>
       <c r="E210" s="4"/>
@@ -3591,7 +3591,7 @@
     </row>
     <row r="211" ht="15.75" customHeight="1">
       <c r="A211" s="22"/>
-      <c r="B211" s="23"/>
+      <c r="B211" s="21"/>
       <c r="C211" s="4"/>
       <c r="D211" s="4"/>
       <c r="E211" s="4"/>
@@ -3601,7 +3601,7 @@
     </row>
     <row r="212" ht="15.75" customHeight="1">
       <c r="A212" s="22"/>
-      <c r="B212" s="23"/>
+      <c r="B212" s="21"/>
       <c r="C212" s="4"/>
       <c r="D212" s="4"/>
       <c r="E212" s="4"/>
@@ -3611,7 +3611,7 @@
     </row>
     <row r="213" ht="15.75" customHeight="1">
       <c r="A213" s="22"/>
-      <c r="B213" s="23"/>
+      <c r="B213" s="21"/>
       <c r="C213" s="4"/>
       <c r="D213" s="4"/>
       <c r="E213" s="4"/>
@@ -3621,7 +3621,7 @@
     </row>
     <row r="214" ht="15.75" customHeight="1">
       <c r="A214" s="22"/>
-      <c r="B214" s="23"/>
+      <c r="B214" s="21"/>
       <c r="C214" s="4"/>
       <c r="D214" s="4"/>
       <c r="E214" s="4"/>
@@ -3631,7 +3631,7 @@
     </row>
     <row r="215" ht="15.75" customHeight="1">
       <c r="A215" s="22"/>
-      <c r="B215" s="23"/>
+      <c r="B215" s="21"/>
       <c r="C215" s="4"/>
       <c r="D215" s="4"/>
       <c r="E215" s="4"/>
@@ -3641,7 +3641,7 @@
     </row>
     <row r="216" ht="15.75" customHeight="1">
       <c r="A216" s="22"/>
-      <c r="B216" s="23"/>
+      <c r="B216" s="21"/>
       <c r="C216" s="4"/>
       <c r="D216" s="4"/>
       <c r="E216" s="4"/>
@@ -3651,7 +3651,7 @@
     </row>
     <row r="217" ht="15.75" customHeight="1">
       <c r="A217" s="22"/>
-      <c r="B217" s="23"/>
+      <c r="B217" s="21"/>
       <c r="C217" s="4"/>
       <c r="D217" s="4"/>
       <c r="E217" s="4"/>
@@ -3661,7 +3661,7 @@
     </row>
     <row r="218" ht="15.75" customHeight="1">
       <c r="A218" s="22"/>
-      <c r="B218" s="23"/>
+      <c r="B218" s="21"/>
       <c r="C218" s="4"/>
       <c r="D218" s="4"/>
       <c r="E218" s="4"/>
@@ -3671,7 +3671,7 @@
     </row>
     <row r="219" ht="15.75" customHeight="1">
       <c r="A219" s="22"/>
-      <c r="B219" s="23"/>
+      <c r="B219" s="21"/>
       <c r="C219" s="4"/>
       <c r="D219" s="4"/>
       <c r="E219" s="4"/>
@@ -3681,7 +3681,7 @@
     </row>
     <row r="220" ht="15.75" customHeight="1">
       <c r="A220" s="22"/>
-      <c r="B220" s="23"/>
+      <c r="B220" s="21"/>
       <c r="C220" s="4"/>
       <c r="D220" s="4"/>
       <c r="E220" s="4"/>
@@ -4560,8 +4560,11 @@
       <c r="H307" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A307">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A120">
+      <formula1>",Add to project and/or study,Remove from project,Remove from study"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A121:A307">
       <formula1>"Add,Remove"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4581,13 +4584,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.3516" style="24" customWidth="1"/>
-    <col min="2" max="5" width="9.35156" style="24" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="24" customWidth="1"/>
+    <col min="1" max="1" width="26.4375" style="23" customWidth="1"/>
+    <col min="2" max="5" width="9.35156" style="23" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" t="s" s="25">
+      <c r="A1" t="s" s="24">
         <v>5</v>
       </c>
       <c r="B1" s="4"/>
@@ -4614,91 +4617,93 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="21"/>
+      <c r="A4" t="s" s="19">
+        <v>23</v>
+      </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="21"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="21"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="21"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="21"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="21"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="21"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="21"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="21"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="21"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="21"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
     <row r="15" ht="15" customHeight="1">
-      <c r="A15" s="21"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="21"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>

</xml_diff>